<commit_message>
done with most coding, ready to finish paper
</commit_message>
<xml_diff>
--- a/model_eval.xlsx
+++ b/model_eval.xlsx
@@ -226,6 +226,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$C$3:$C$22</c:f>
@@ -335,6 +404,75 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$D$3:$D$22</c:f>
@@ -432,6 +570,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$F$3:$F$22</c:f>
@@ -529,6 +736,75 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$H$3:$H$22</c:f>
@@ -619,6 +895,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>

</xml_diff>